<commit_message>
organize data for development, create enum to make data fetching consistent, create first tests
</commit_message>
<xml_diff>
--- a/public/data/data.xlsx
+++ b/public/data/data.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29721"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10208"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuni-my.sharepoint.com/personal/henriikka_meskanen_tuni_fi/Documents/4. vuosi/LOG.720_Tiedeklinikka/DATA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurapihamaa/lukina/public/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D64FFDC8-7937-4119-AD47-021D7F4C6542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB9DAAF1-D3E3-4B40-8C0D-35D8A10F1B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32680" yWindow="3100" windowWidth="23260" windowHeight="12460" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
+    <sheet name="Taul2" sheetId="2" r:id="rId2"/>
+    <sheet name="Taul3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="81">
   <si>
     <t>Virheetön teksti</t>
   </si>
@@ -2017,7 +2019,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2127,7 +2129,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normaali" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2405,22 +2407,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E412"/>
+  <dimension ref="A1:E407"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView zoomScale="88" workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="64.140625" customWidth="1"/>
-    <col min="2" max="2" width="59.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1"/>
-    <col min="5" max="5" width="26.5703125" customWidth="1"/>
+    <col min="1" max="1" width="64.1640625" customWidth="1"/>
+    <col min="2" max="2" width="59.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
+    <col min="5" max="5" width="26.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.9">
+    <row r="1" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2437,7 +2439,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>5</v>
       </c>
@@ -2454,7 +2456,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="28.9">
+    <row r="3" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>9</v>
       </c>
@@ -2471,7 +2473,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="43.15">
+    <row r="4" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>13</v>
       </c>
@@ -2488,7 +2490,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="28.9">
+    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -2505,7 +2507,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="28.9">
+    <row r="6" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>21</v>
       </c>
@@ -2522,7 +2524,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="28.9">
+    <row r="7" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>25</v>
       </c>
@@ -2539,7 +2541,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="28.9">
+    <row r="8" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>29</v>
       </c>
@@ -2556,7 +2558,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="28.9">
+    <row r="9" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>33</v>
       </c>
@@ -2573,7 +2575,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="43.15">
+    <row r="10" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>37</v>
       </c>
@@ -2590,7 +2592,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="28.9">
+    <row r="11" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>41</v>
       </c>
@@ -2607,2266 +2609,2153 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="43.15">
-      <c r="A12" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>46</v>
+    <row r="12" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>54</v>
       </c>
       <c r="C12" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="43.15">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="C13" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="28.9">
-      <c r="A14" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14" s="1">
-        <v>3</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="43.15">
-      <c r="A15" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" s="1">
-        <v>5</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="72">
-      <c r="A16" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C16" s="1">
-        <v>6</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="57.6">
-      <c r="A17" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C17" s="1">
-        <v>2</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E17" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="57.6">
-      <c r="A18" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C18" s="1">
-        <v>5</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="72">
-      <c r="A19" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="C19" s="1">
-        <v>8</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="302.45" customHeight="1">
-      <c r="A20" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C20" s="1">
-        <v>16</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B14"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B15"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" ht="302.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="1"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="1"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="1"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="1"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="1"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="1"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="1"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="1"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
     </row>
-    <row r="75" spans="1:5">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="1"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="1"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="1"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="1"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
       <c r="E80" s="1"/>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
     </row>
-    <row r="82" spans="1:5">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
       <c r="E82" s="1"/>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="1"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
       <c r="E83" s="1"/>
     </row>
-    <row r="84" spans="1:5">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="1"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
     </row>
-    <row r="85" spans="1:5">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="1"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="1"/>
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="1"/>
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="1"/>
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="1"/>
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
     </row>
-    <row r="90" spans="1:5">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" s="1"/>
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" s="1"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" s="1"/>
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
     </row>
-    <row r="93" spans="1:5">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" s="1"/>
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
       <c r="E93" s="1"/>
     </row>
-    <row r="94" spans="1:5">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" s="1"/>
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
       <c r="E94" s="1"/>
     </row>
-    <row r="95" spans="1:5">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" s="1"/>
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
       <c r="E95" s="1"/>
     </row>
-    <row r="96" spans="1:5">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" s="1"/>
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
       <c r="E96" s="1"/>
     </row>
-    <row r="97" spans="1:5">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" s="1"/>
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>
       <c r="E97" s="1"/>
     </row>
-    <row r="98" spans="1:5">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" s="1"/>
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
       <c r="E98" s="1"/>
     </row>
-    <row r="99" spans="1:5">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" s="1"/>
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
       <c r="E99" s="1"/>
     </row>
-    <row r="100" spans="1:5">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" s="1"/>
       <c r="C100" s="1"/>
       <c r="D100" s="1"/>
       <c r="E100" s="1"/>
     </row>
-    <row r="101" spans="1:5">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" s="1"/>
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
       <c r="E101" s="1"/>
     </row>
-    <row r="102" spans="1:5">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" s="1"/>
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
       <c r="E102" s="1"/>
     </row>
-    <row r="103" spans="1:5">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" s="1"/>
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
       <c r="E103" s="1"/>
     </row>
-    <row r="104" spans="1:5">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" s="1"/>
       <c r="C104" s="1"/>
       <c r="D104" s="1"/>
       <c r="E104" s="1"/>
     </row>
-    <row r="105" spans="1:5">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" s="1"/>
       <c r="C105" s="1"/>
       <c r="D105" s="1"/>
       <c r="E105" s="1"/>
     </row>
-    <row r="106" spans="1:5">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" s="1"/>
       <c r="C106" s="1"/>
       <c r="D106" s="1"/>
       <c r="E106" s="1"/>
     </row>
-    <row r="107" spans="1:5">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" s="1"/>
       <c r="C107" s="1"/>
       <c r="D107" s="1"/>
       <c r="E107" s="1"/>
     </row>
-    <row r="108" spans="1:5">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" s="1"/>
       <c r="C108" s="1"/>
       <c r="D108" s="1"/>
       <c r="E108" s="1"/>
     </row>
-    <row r="109" spans="1:5">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" s="1"/>
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
       <c r="E109" s="1"/>
     </row>
-    <row r="110" spans="1:5">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" s="1"/>
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
       <c r="E110" s="1"/>
     </row>
-    <row r="111" spans="1:5">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" s="1"/>
       <c r="C111" s="1"/>
       <c r="D111" s="1"/>
       <c r="E111" s="1"/>
     </row>
-    <row r="112" spans="1:5">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" s="1"/>
       <c r="C112" s="1"/>
       <c r="D112" s="1"/>
       <c r="E112" s="1"/>
     </row>
-    <row r="113" spans="1:5">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" s="1"/>
       <c r="C113" s="1"/>
       <c r="D113" s="1"/>
       <c r="E113" s="1"/>
     </row>
-    <row r="114" spans="1:5">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" s="1"/>
       <c r="C114" s="1"/>
       <c r="D114" s="1"/>
       <c r="E114" s="1"/>
     </row>
-    <row r="115" spans="1:5">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" s="1"/>
       <c r="C115" s="1"/>
       <c r="D115" s="1"/>
       <c r="E115" s="1"/>
     </row>
-    <row r="116" spans="1:5">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" s="1"/>
       <c r="C116" s="1"/>
       <c r="D116" s="1"/>
       <c r="E116" s="1"/>
     </row>
-    <row r="117" spans="1:5">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" s="1"/>
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
       <c r="E117" s="1"/>
     </row>
-    <row r="118" spans="1:5">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" s="1"/>
       <c r="C118" s="1"/>
       <c r="D118" s="1"/>
       <c r="E118" s="1"/>
     </row>
-    <row r="119" spans="1:5">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" s="1"/>
       <c r="C119" s="1"/>
       <c r="D119" s="1"/>
       <c r="E119" s="1"/>
     </row>
-    <row r="120" spans="1:5">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" s="1"/>
       <c r="C120" s="1"/>
       <c r="D120" s="1"/>
       <c r="E120" s="1"/>
     </row>
-    <row r="121" spans="1:5">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" s="1"/>
       <c r="C121" s="1"/>
       <c r="D121" s="1"/>
       <c r="E121" s="1"/>
     </row>
-    <row r="122" spans="1:5">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" s="1"/>
       <c r="C122" s="1"/>
       <c r="D122" s="1"/>
       <c r="E122" s="1"/>
     </row>
-    <row r="123" spans="1:5">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" s="1"/>
       <c r="C123" s="1"/>
       <c r="D123" s="1"/>
       <c r="E123" s="1"/>
     </row>
-    <row r="124" spans="1:5">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" s="1"/>
       <c r="C124" s="1"/>
       <c r="D124" s="1"/>
       <c r="E124" s="1"/>
     </row>
-    <row r="125" spans="1:5">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" s="1"/>
       <c r="C125" s="1"/>
       <c r="D125" s="1"/>
       <c r="E125" s="1"/>
     </row>
-    <row r="126" spans="1:5">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" s="1"/>
       <c r="C126" s="1"/>
       <c r="D126" s="1"/>
       <c r="E126" s="1"/>
     </row>
-    <row r="127" spans="1:5">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" s="1"/>
       <c r="C127" s="1"/>
       <c r="D127" s="1"/>
       <c r="E127" s="1"/>
     </row>
-    <row r="128" spans="1:5">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" s="1"/>
       <c r="C128" s="1"/>
       <c r="D128" s="1"/>
       <c r="E128" s="1"/>
     </row>
-    <row r="129" spans="1:5">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A129" s="1"/>
       <c r="C129" s="1"/>
       <c r="D129" s="1"/>
       <c r="E129" s="1"/>
     </row>
-    <row r="130" spans="1:5">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A130" s="1"/>
       <c r="C130" s="1"/>
       <c r="D130" s="1"/>
       <c r="E130" s="1"/>
     </row>
-    <row r="131" spans="1:5">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A131" s="1"/>
       <c r="C131" s="1"/>
       <c r="D131" s="1"/>
       <c r="E131" s="1"/>
     </row>
-    <row r="132" spans="1:5">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A132" s="1"/>
       <c r="C132" s="1"/>
       <c r="D132" s="1"/>
       <c r="E132" s="1"/>
     </row>
-    <row r="133" spans="1:5">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A133" s="1"/>
       <c r="C133" s="1"/>
       <c r="D133" s="1"/>
       <c r="E133" s="1"/>
     </row>
-    <row r="134" spans="1:5">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A134" s="1"/>
       <c r="C134" s="1"/>
       <c r="D134" s="1"/>
       <c r="E134" s="1"/>
     </row>
-    <row r="135" spans="1:5">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A135" s="1"/>
       <c r="C135" s="1"/>
       <c r="D135" s="1"/>
       <c r="E135" s="1"/>
     </row>
-    <row r="136" spans="1:5">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A136" s="1"/>
       <c r="C136" s="1"/>
       <c r="D136" s="1"/>
       <c r="E136" s="1"/>
     </row>
-    <row r="137" spans="1:5">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A137" s="1"/>
       <c r="C137" s="1"/>
       <c r="D137" s="1"/>
       <c r="E137" s="1"/>
     </row>
-    <row r="138" spans="1:5">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A138" s="1"/>
       <c r="C138" s="1"/>
       <c r="D138" s="1"/>
       <c r="E138" s="1"/>
     </row>
-    <row r="139" spans="1:5">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A139" s="1"/>
       <c r="C139" s="1"/>
       <c r="D139" s="1"/>
       <c r="E139" s="1"/>
     </row>
-    <row r="140" spans="1:5">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A140" s="1"/>
       <c r="C140" s="1"/>
       <c r="D140" s="1"/>
       <c r="E140" s="1"/>
     </row>
-    <row r="141" spans="1:5">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A141" s="1"/>
       <c r="C141" s="1"/>
       <c r="D141" s="1"/>
       <c r="E141" s="1"/>
     </row>
-    <row r="142" spans="1:5">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A142" s="1"/>
       <c r="C142" s="1"/>
       <c r="D142" s="1"/>
       <c r="E142" s="1"/>
     </row>
-    <row r="143" spans="1:5">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A143" s="1"/>
       <c r="C143" s="1"/>
       <c r="D143" s="1"/>
       <c r="E143" s="1"/>
     </row>
-    <row r="144" spans="1:5">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A144" s="1"/>
       <c r="C144" s="1"/>
       <c r="D144" s="1"/>
       <c r="E144" s="1"/>
     </row>
-    <row r="145" spans="1:5">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A145" s="1"/>
       <c r="C145" s="1"/>
       <c r="D145" s="1"/>
       <c r="E145" s="1"/>
     </row>
-    <row r="146" spans="1:5">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A146" s="1"/>
       <c r="C146" s="1"/>
       <c r="D146" s="1"/>
       <c r="E146" s="1"/>
     </row>
-    <row r="147" spans="1:5">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A147" s="1"/>
       <c r="C147" s="1"/>
       <c r="D147" s="1"/>
       <c r="E147" s="1"/>
     </row>
-    <row r="148" spans="1:5">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A148" s="1"/>
       <c r="C148" s="1"/>
       <c r="D148" s="1"/>
       <c r="E148" s="1"/>
     </row>
-    <row r="149" spans="1:5">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A149" s="1"/>
       <c r="C149" s="1"/>
       <c r="D149" s="1"/>
       <c r="E149" s="1"/>
     </row>
-    <row r="150" spans="1:5">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A150" s="1"/>
       <c r="C150" s="1"/>
       <c r="D150" s="1"/>
       <c r="E150" s="1"/>
     </row>
-    <row r="151" spans="1:5">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A151" s="1"/>
       <c r="C151" s="1"/>
       <c r="D151" s="1"/>
       <c r="E151" s="1"/>
     </row>
-    <row r="152" spans="1:5">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A152" s="1"/>
       <c r="C152" s="1"/>
       <c r="D152" s="1"/>
       <c r="E152" s="1"/>
     </row>
-    <row r="153" spans="1:5">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A153" s="1"/>
       <c r="C153" s="1"/>
       <c r="D153" s="1"/>
       <c r="E153" s="1"/>
     </row>
-    <row r="154" spans="1:5">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A154" s="1"/>
       <c r="C154" s="1"/>
       <c r="D154" s="1"/>
       <c r="E154" s="1"/>
     </row>
-    <row r="155" spans="1:5">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" s="1"/>
       <c r="C155" s="1"/>
       <c r="D155" s="1"/>
       <c r="E155" s="1"/>
     </row>
-    <row r="156" spans="1:5">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A156" s="1"/>
       <c r="C156" s="1"/>
       <c r="D156" s="1"/>
       <c r="E156" s="1"/>
     </row>
-    <row r="157" spans="1:5">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A157" s="1"/>
       <c r="C157" s="1"/>
       <c r="D157" s="1"/>
       <c r="E157" s="1"/>
     </row>
-    <row r="158" spans="1:5">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A158" s="1"/>
       <c r="C158" s="1"/>
       <c r="D158" s="1"/>
       <c r="E158" s="1"/>
     </row>
-    <row r="159" spans="1:5">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A159" s="1"/>
       <c r="C159" s="1"/>
       <c r="D159" s="1"/>
       <c r="E159" s="1"/>
     </row>
-    <row r="160" spans="1:5">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A160" s="1"/>
       <c r="C160" s="1"/>
       <c r="D160" s="1"/>
       <c r="E160" s="1"/>
     </row>
-    <row r="161" spans="1:5">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A161" s="1"/>
       <c r="C161" s="1"/>
       <c r="D161" s="1"/>
       <c r="E161" s="1"/>
     </row>
-    <row r="162" spans="1:5">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A162" s="1"/>
       <c r="C162" s="1"/>
       <c r="D162" s="1"/>
       <c r="E162" s="1"/>
     </row>
-    <row r="163" spans="1:5">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A163" s="1"/>
       <c r="C163" s="1"/>
       <c r="D163" s="1"/>
       <c r="E163" s="1"/>
     </row>
-    <row r="164" spans="1:5">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A164" s="1"/>
       <c r="C164" s="1"/>
       <c r="D164" s="1"/>
       <c r="E164" s="1"/>
     </row>
-    <row r="165" spans="1:5">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A165" s="1"/>
       <c r="C165" s="1"/>
       <c r="D165" s="1"/>
       <c r="E165" s="1"/>
     </row>
-    <row r="166" spans="1:5">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A166" s="1"/>
       <c r="C166" s="1"/>
       <c r="D166" s="1"/>
       <c r="E166" s="1"/>
     </row>
-    <row r="167" spans="1:5">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A167" s="1"/>
       <c r="C167" s="1"/>
       <c r="D167" s="1"/>
       <c r="E167" s="1"/>
     </row>
-    <row r="168" spans="1:5">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A168" s="1"/>
       <c r="C168" s="1"/>
       <c r="D168" s="1"/>
       <c r="E168" s="1"/>
     </row>
-    <row r="169" spans="1:5">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A169" s="1"/>
       <c r="C169" s="1"/>
       <c r="D169" s="1"/>
       <c r="E169" s="1"/>
     </row>
-    <row r="170" spans="1:5">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A170" s="1"/>
       <c r="C170" s="1"/>
       <c r="D170" s="1"/>
       <c r="E170" s="1"/>
     </row>
-    <row r="171" spans="1:5">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A171" s="1"/>
       <c r="C171" s="1"/>
       <c r="D171" s="1"/>
       <c r="E171" s="1"/>
     </row>
-    <row r="172" spans="1:5">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A172" s="1"/>
       <c r="C172" s="1"/>
       <c r="D172" s="1"/>
       <c r="E172" s="1"/>
     </row>
-    <row r="173" spans="1:5">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A173" s="1"/>
       <c r="C173" s="1"/>
       <c r="D173" s="1"/>
       <c r="E173" s="1"/>
     </row>
-    <row r="174" spans="1:5">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A174" s="1"/>
       <c r="C174" s="1"/>
       <c r="D174" s="1"/>
       <c r="E174" s="1"/>
     </row>
-    <row r="175" spans="1:5">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A175" s="1"/>
       <c r="C175" s="1"/>
       <c r="D175" s="1"/>
       <c r="E175" s="1"/>
     </row>
-    <row r="176" spans="1:5">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A176" s="1"/>
       <c r="C176" s="1"/>
       <c r="D176" s="1"/>
       <c r="E176" s="1"/>
     </row>
-    <row r="177" spans="1:5">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A177" s="1"/>
       <c r="C177" s="1"/>
       <c r="D177" s="1"/>
       <c r="E177" s="1"/>
     </row>
-    <row r="178" spans="1:5">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A178" s="1"/>
       <c r="C178" s="1"/>
       <c r="D178" s="1"/>
       <c r="E178" s="1"/>
     </row>
-    <row r="179" spans="1:5">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A179" s="1"/>
       <c r="C179" s="1"/>
       <c r="D179" s="1"/>
       <c r="E179" s="1"/>
     </row>
-    <row r="180" spans="1:5">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A180" s="1"/>
       <c r="C180" s="1"/>
       <c r="D180" s="1"/>
       <c r="E180" s="1"/>
     </row>
-    <row r="181" spans="1:5">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A181" s="1"/>
       <c r="C181" s="1"/>
       <c r="D181" s="1"/>
       <c r="E181" s="1"/>
     </row>
-    <row r="182" spans="1:5">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A182" s="1"/>
       <c r="C182" s="1"/>
       <c r="D182" s="1"/>
       <c r="E182" s="1"/>
     </row>
-    <row r="183" spans="1:5">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A183" s="1"/>
       <c r="C183" s="1"/>
       <c r="D183" s="1"/>
       <c r="E183" s="1"/>
     </row>
-    <row r="184" spans="1:5">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A184" s="1"/>
       <c r="C184" s="1"/>
       <c r="D184" s="1"/>
       <c r="E184" s="1"/>
     </row>
-    <row r="185" spans="1:5">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A185" s="1"/>
       <c r="C185" s="1"/>
       <c r="D185" s="1"/>
       <c r="E185" s="1"/>
     </row>
-    <row r="186" spans="1:5">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A186" s="1"/>
       <c r="C186" s="1"/>
       <c r="D186" s="1"/>
       <c r="E186" s="1"/>
     </row>
-    <row r="187" spans="1:5">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A187" s="1"/>
       <c r="C187" s="1"/>
       <c r="D187" s="1"/>
       <c r="E187" s="1"/>
     </row>
-    <row r="188" spans="1:5">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A188" s="1"/>
       <c r="C188" s="1"/>
       <c r="D188" s="1"/>
       <c r="E188" s="1"/>
     </row>
-    <row r="189" spans="1:5">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A189" s="1"/>
       <c r="C189" s="1"/>
       <c r="D189" s="1"/>
       <c r="E189" s="1"/>
     </row>
-    <row r="190" spans="1:5">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A190" s="1"/>
       <c r="C190" s="1"/>
       <c r="D190" s="1"/>
       <c r="E190" s="1"/>
     </row>
-    <row r="191" spans="1:5">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A191" s="1"/>
       <c r="C191" s="1"/>
       <c r="D191" s="1"/>
       <c r="E191" s="1"/>
     </row>
-    <row r="192" spans="1:5">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A192" s="1"/>
       <c r="C192" s="1"/>
       <c r="D192" s="1"/>
       <c r="E192" s="1"/>
     </row>
-    <row r="193" spans="1:5">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A193" s="1"/>
       <c r="C193" s="1"/>
       <c r="D193" s="1"/>
       <c r="E193" s="1"/>
     </row>
-    <row r="194" spans="1:5">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A194" s="1"/>
       <c r="C194" s="1"/>
       <c r="D194" s="1"/>
       <c r="E194" s="1"/>
     </row>
-    <row r="195" spans="1:5">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A195" s="1"/>
       <c r="C195" s="1"/>
       <c r="D195" s="1"/>
       <c r="E195" s="1"/>
     </row>
-    <row r="196" spans="1:5">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A196" s="1"/>
       <c r="C196" s="1"/>
       <c r="D196" s="1"/>
       <c r="E196" s="1"/>
     </row>
-    <row r="197" spans="1:5">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A197" s="1"/>
       <c r="C197" s="1"/>
       <c r="D197" s="1"/>
       <c r="E197" s="1"/>
     </row>
-    <row r="198" spans="1:5">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A198" s="1"/>
       <c r="C198" s="1"/>
       <c r="D198" s="1"/>
       <c r="E198" s="1"/>
     </row>
-    <row r="199" spans="1:5">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A199" s="1"/>
       <c r="C199" s="1"/>
       <c r="D199" s="1"/>
       <c r="E199" s="1"/>
     </row>
-    <row r="200" spans="1:5">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A200" s="1"/>
       <c r="C200" s="1"/>
       <c r="D200" s="1"/>
       <c r="E200" s="1"/>
     </row>
-    <row r="201" spans="1:5">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A201" s="1"/>
       <c r="C201" s="1"/>
       <c r="D201" s="1"/>
       <c r="E201" s="1"/>
     </row>
-    <row r="202" spans="1:5">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A202" s="1"/>
       <c r="C202" s="1"/>
       <c r="D202" s="1"/>
       <c r="E202" s="1"/>
     </row>
-    <row r="203" spans="1:5">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A203" s="1"/>
       <c r="C203" s="1"/>
       <c r="D203" s="1"/>
       <c r="E203" s="1"/>
     </row>
-    <row r="204" spans="1:5">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A204" s="1"/>
       <c r="C204" s="1"/>
       <c r="D204" s="1"/>
       <c r="E204" s="1"/>
     </row>
-    <row r="205" spans="1:5">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A205" s="1"/>
       <c r="C205" s="1"/>
       <c r="D205" s="1"/>
       <c r="E205" s="1"/>
     </row>
-    <row r="206" spans="1:5">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A206" s="1"/>
       <c r="C206" s="1"/>
       <c r="D206" s="1"/>
       <c r="E206" s="1"/>
     </row>
-    <row r="207" spans="1:5">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A207" s="1"/>
       <c r="C207" s="1"/>
       <c r="D207" s="1"/>
       <c r="E207" s="1"/>
     </row>
-    <row r="208" spans="1:5">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A208" s="1"/>
       <c r="C208" s="1"/>
       <c r="D208" s="1"/>
       <c r="E208" s="1"/>
     </row>
-    <row r="209" spans="1:5">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A209" s="1"/>
       <c r="C209" s="1"/>
       <c r="D209" s="1"/>
       <c r="E209" s="1"/>
     </row>
-    <row r="210" spans="1:5">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A210" s="1"/>
       <c r="C210" s="1"/>
       <c r="D210" s="1"/>
       <c r="E210" s="1"/>
     </row>
-    <row r="211" spans="1:5">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A211" s="1"/>
       <c r="C211" s="1"/>
       <c r="D211" s="1"/>
       <c r="E211" s="1"/>
     </row>
-    <row r="212" spans="1:5">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A212" s="1"/>
       <c r="C212" s="1"/>
       <c r="D212" s="1"/>
       <c r="E212" s="1"/>
     </row>
-    <row r="213" spans="1:5">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A213" s="1"/>
       <c r="C213" s="1"/>
       <c r="D213" s="1"/>
       <c r="E213" s="1"/>
     </row>
-    <row r="214" spans="1:5">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A214" s="1"/>
       <c r="C214" s="1"/>
       <c r="D214" s="1"/>
       <c r="E214" s="1"/>
     </row>
-    <row r="215" spans="1:5">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A215" s="1"/>
       <c r="C215" s="1"/>
       <c r="D215" s="1"/>
       <c r="E215" s="1"/>
     </row>
-    <row r="216" spans="1:5">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A216" s="1"/>
       <c r="C216" s="1"/>
       <c r="D216" s="1"/>
       <c r="E216" s="1"/>
     </row>
-    <row r="217" spans="1:5">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A217" s="1"/>
       <c r="C217" s="1"/>
       <c r="D217" s="1"/>
       <c r="E217" s="1"/>
     </row>
-    <row r="218" spans="1:5">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A218" s="1"/>
       <c r="C218" s="1"/>
       <c r="D218" s="1"/>
       <c r="E218" s="1"/>
     </row>
-    <row r="219" spans="1:5">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A219" s="1"/>
       <c r="C219" s="1"/>
       <c r="D219" s="1"/>
       <c r="E219" s="1"/>
     </row>
-    <row r="220" spans="1:5">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A220" s="1"/>
       <c r="C220" s="1"/>
       <c r="D220" s="1"/>
       <c r="E220" s="1"/>
     </row>
-    <row r="221" spans="1:5">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A221" s="1"/>
       <c r="C221" s="1"/>
       <c r="D221" s="1"/>
       <c r="E221" s="1"/>
     </row>
-    <row r="222" spans="1:5">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A222" s="1"/>
       <c r="C222" s="1"/>
       <c r="D222" s="1"/>
       <c r="E222" s="1"/>
     </row>
-    <row r="223" spans="1:5">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A223" s="1"/>
       <c r="C223" s="1"/>
       <c r="D223" s="1"/>
       <c r="E223" s="1"/>
     </row>
-    <row r="224" spans="1:5">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A224" s="1"/>
       <c r="C224" s="1"/>
       <c r="D224" s="1"/>
       <c r="E224" s="1"/>
     </row>
-    <row r="225" spans="1:5">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A225" s="1"/>
       <c r="C225" s="1"/>
       <c r="D225" s="1"/>
       <c r="E225" s="1"/>
     </row>
-    <row r="226" spans="1:5">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A226" s="1"/>
       <c r="C226" s="1"/>
       <c r="D226" s="1"/>
       <c r="E226" s="1"/>
     </row>
-    <row r="227" spans="1:5">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A227" s="1"/>
       <c r="C227" s="1"/>
       <c r="D227" s="1"/>
       <c r="E227" s="1"/>
     </row>
-    <row r="228" spans="1:5">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A228" s="1"/>
       <c r="C228" s="1"/>
       <c r="D228" s="1"/>
       <c r="E228" s="1"/>
     </row>
-    <row r="229" spans="1:5">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A229" s="1"/>
       <c r="C229" s="1"/>
       <c r="D229" s="1"/>
       <c r="E229" s="1"/>
     </row>
-    <row r="230" spans="1:5">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A230" s="1"/>
       <c r="C230" s="1"/>
       <c r="D230" s="1"/>
       <c r="E230" s="1"/>
     </row>
-    <row r="231" spans="1:5">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A231" s="1"/>
       <c r="C231" s="1"/>
       <c r="D231" s="1"/>
       <c r="E231" s="1"/>
     </row>
-    <row r="232" spans="1:5">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A232" s="1"/>
       <c r="C232" s="1"/>
       <c r="D232" s="1"/>
       <c r="E232" s="1"/>
     </row>
-    <row r="233" spans="1:5">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A233" s="1"/>
       <c r="C233" s="1"/>
       <c r="D233" s="1"/>
       <c r="E233" s="1"/>
     </row>
-    <row r="234" spans="1:5">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A234" s="1"/>
       <c r="C234" s="1"/>
       <c r="D234" s="1"/>
       <c r="E234" s="1"/>
     </row>
-    <row r="235" spans="1:5">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A235" s="1"/>
       <c r="C235" s="1"/>
       <c r="D235" s="1"/>
       <c r="E235" s="1"/>
     </row>
-    <row r="236" spans="1:5">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A236" s="1"/>
       <c r="C236" s="1"/>
       <c r="D236" s="1"/>
       <c r="E236" s="1"/>
     </row>
-    <row r="237" spans="1:5">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A237" s="1"/>
       <c r="C237" s="1"/>
       <c r="D237" s="1"/>
       <c r="E237" s="1"/>
     </row>
-    <row r="238" spans="1:5">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A238" s="1"/>
       <c r="C238" s="1"/>
       <c r="D238" s="1"/>
       <c r="E238" s="1"/>
     </row>
-    <row r="239" spans="1:5">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A239" s="1"/>
       <c r="C239" s="1"/>
       <c r="D239" s="1"/>
       <c r="E239" s="1"/>
     </row>
-    <row r="240" spans="1:5">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A240" s="1"/>
       <c r="C240" s="1"/>
       <c r="D240" s="1"/>
       <c r="E240" s="1"/>
     </row>
-    <row r="241" spans="1:5">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A241" s="1"/>
       <c r="C241" s="1"/>
       <c r="D241" s="1"/>
       <c r="E241" s="1"/>
     </row>
-    <row r="242" spans="1:5">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A242" s="1"/>
       <c r="C242" s="1"/>
       <c r="D242" s="1"/>
       <c r="E242" s="1"/>
     </row>
-    <row r="243" spans="1:5">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A243" s="1"/>
       <c r="C243" s="1"/>
       <c r="D243" s="1"/>
       <c r="E243" s="1"/>
     </row>
-    <row r="244" spans="1:5">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A244" s="1"/>
       <c r="C244" s="1"/>
       <c r="D244" s="1"/>
       <c r="E244" s="1"/>
     </row>
-    <row r="245" spans="1:5">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A245" s="1"/>
       <c r="C245" s="1"/>
       <c r="D245" s="1"/>
       <c r="E245" s="1"/>
     </row>
-    <row r="246" spans="1:5">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A246" s="1"/>
       <c r="C246" s="1"/>
       <c r="D246" s="1"/>
       <c r="E246" s="1"/>
     </row>
-    <row r="247" spans="1:5">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A247" s="1"/>
       <c r="C247" s="1"/>
       <c r="D247" s="1"/>
       <c r="E247" s="1"/>
     </row>
-    <row r="248" spans="1:5">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A248" s="1"/>
       <c r="C248" s="1"/>
       <c r="D248" s="1"/>
       <c r="E248" s="1"/>
     </row>
-    <row r="249" spans="1:5">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A249" s="1"/>
       <c r="C249" s="1"/>
       <c r="D249" s="1"/>
       <c r="E249" s="1"/>
     </row>
-    <row r="250" spans="1:5">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A250" s="1"/>
       <c r="C250" s="1"/>
       <c r="D250" s="1"/>
       <c r="E250" s="1"/>
     </row>
-    <row r="251" spans="1:5">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A251" s="1"/>
       <c r="C251" s="1"/>
       <c r="D251" s="1"/>
       <c r="E251" s="1"/>
     </row>
-    <row r="252" spans="1:5">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A252" s="1"/>
       <c r="C252" s="1"/>
       <c r="D252" s="1"/>
       <c r="E252" s="1"/>
     </row>
-    <row r="253" spans="1:5">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A253" s="1"/>
       <c r="C253" s="1"/>
       <c r="D253" s="1"/>
       <c r="E253" s="1"/>
     </row>
-    <row r="254" spans="1:5">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A254" s="1"/>
       <c r="C254" s="1"/>
       <c r="D254" s="1"/>
       <c r="E254" s="1"/>
     </row>
-    <row r="255" spans="1:5">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A255" s="1"/>
       <c r="C255" s="1"/>
       <c r="D255" s="1"/>
       <c r="E255" s="1"/>
     </row>
-    <row r="256" spans="1:5">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A256" s="1"/>
       <c r="C256" s="1"/>
       <c r="D256" s="1"/>
       <c r="E256" s="1"/>
     </row>
-    <row r="257" spans="1:5">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A257" s="1"/>
       <c r="C257" s="1"/>
       <c r="D257" s="1"/>
       <c r="E257" s="1"/>
     </row>
-    <row r="258" spans="1:5">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A258" s="1"/>
       <c r="C258" s="1"/>
       <c r="D258" s="1"/>
       <c r="E258" s="1"/>
     </row>
-    <row r="259" spans="1:5">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A259" s="1"/>
       <c r="C259" s="1"/>
       <c r="D259" s="1"/>
       <c r="E259" s="1"/>
     </row>
-    <row r="260" spans="1:5">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A260" s="1"/>
       <c r="C260" s="1"/>
       <c r="D260" s="1"/>
       <c r="E260" s="1"/>
     </row>
-    <row r="261" spans="1:5">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A261" s="1"/>
       <c r="C261" s="1"/>
       <c r="D261" s="1"/>
       <c r="E261" s="1"/>
     </row>
-    <row r="262" spans="1:5">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A262" s="1"/>
       <c r="C262" s="1"/>
       <c r="D262" s="1"/>
       <c r="E262" s="1"/>
     </row>
-    <row r="263" spans="1:5">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A263" s="1"/>
       <c r="C263" s="1"/>
       <c r="D263" s="1"/>
       <c r="E263" s="1"/>
     </row>
-    <row r="264" spans="1:5">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A264" s="1"/>
       <c r="C264" s="1"/>
       <c r="D264" s="1"/>
       <c r="E264" s="1"/>
     </row>
-    <row r="265" spans="1:5">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A265" s="1"/>
       <c r="C265" s="1"/>
       <c r="D265" s="1"/>
       <c r="E265" s="1"/>
     </row>
-    <row r="266" spans="1:5">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A266" s="1"/>
       <c r="C266" s="1"/>
       <c r="D266" s="1"/>
       <c r="E266" s="1"/>
     </row>
-    <row r="267" spans="1:5">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A267" s="1"/>
       <c r="C267" s="1"/>
       <c r="D267" s="1"/>
       <c r="E267" s="1"/>
     </row>
-    <row r="268" spans="1:5">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A268" s="1"/>
       <c r="C268" s="1"/>
       <c r="D268" s="1"/>
       <c r="E268" s="1"/>
     </row>
-    <row r="269" spans="1:5">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A269" s="1"/>
       <c r="C269" s="1"/>
       <c r="D269" s="1"/>
       <c r="E269" s="1"/>
     </row>
-    <row r="270" spans="1:5">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A270" s="1"/>
       <c r="C270" s="1"/>
       <c r="D270" s="1"/>
       <c r="E270" s="1"/>
     </row>
-    <row r="271" spans="1:5">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A271" s="1"/>
       <c r="C271" s="1"/>
       <c r="D271" s="1"/>
       <c r="E271" s="1"/>
     </row>
-    <row r="272" spans="1:5">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A272" s="1"/>
       <c r="C272" s="1"/>
       <c r="D272" s="1"/>
       <c r="E272" s="1"/>
     </row>
-    <row r="273" spans="1:5">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A273" s="1"/>
       <c r="C273" s="1"/>
       <c r="D273" s="1"/>
       <c r="E273" s="1"/>
     </row>
-    <row r="274" spans="1:5">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A274" s="1"/>
       <c r="C274" s="1"/>
       <c r="D274" s="1"/>
       <c r="E274" s="1"/>
     </row>
-    <row r="275" spans="1:5">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A275" s="1"/>
       <c r="C275" s="1"/>
       <c r="D275" s="1"/>
       <c r="E275" s="1"/>
     </row>
-    <row r="276" spans="1:5">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A276" s="1"/>
       <c r="C276" s="1"/>
       <c r="D276" s="1"/>
       <c r="E276" s="1"/>
     </row>
-    <row r="277" spans="1:5">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A277" s="1"/>
       <c r="C277" s="1"/>
       <c r="D277" s="1"/>
       <c r="E277" s="1"/>
     </row>
-    <row r="278" spans="1:5">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A278" s="1"/>
       <c r="C278" s="1"/>
       <c r="D278" s="1"/>
       <c r="E278" s="1"/>
     </row>
-    <row r="279" spans="1:5">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A279" s="1"/>
       <c r="C279" s="1"/>
       <c r="D279" s="1"/>
       <c r="E279" s="1"/>
     </row>
-    <row r="280" spans="1:5">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A280" s="1"/>
       <c r="C280" s="1"/>
       <c r="D280" s="1"/>
       <c r="E280" s="1"/>
     </row>
-    <row r="281" spans="1:5">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A281" s="1"/>
       <c r="C281" s="1"/>
       <c r="D281" s="1"/>
       <c r="E281" s="1"/>
     </row>
-    <row r="282" spans="1:5">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A282" s="1"/>
       <c r="C282" s="1"/>
       <c r="D282" s="1"/>
       <c r="E282" s="1"/>
     </row>
-    <row r="283" spans="1:5">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A283" s="1"/>
       <c r="C283" s="1"/>
       <c r="D283" s="1"/>
       <c r="E283" s="1"/>
     </row>
-    <row r="284" spans="1:5">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A284" s="1"/>
       <c r="C284" s="1"/>
       <c r="D284" s="1"/>
       <c r="E284" s="1"/>
     </row>
-    <row r="285" spans="1:5">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A285" s="1"/>
       <c r="C285" s="1"/>
       <c r="D285" s="1"/>
       <c r="E285" s="1"/>
     </row>
-    <row r="286" spans="1:5">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A286" s="1"/>
       <c r="C286" s="1"/>
-      <c r="D286" s="1"/>
-      <c r="E286" s="1"/>
-    </row>
-    <row r="287" spans="1:5">
+    </row>
+    <row r="287" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A287" s="1"/>
       <c r="C287" s="1"/>
-      <c r="D287" s="1"/>
-      <c r="E287" s="1"/>
-    </row>
-    <row r="288" spans="1:5">
+    </row>
+    <row r="288" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A288" s="1"/>
       <c r="C288" s="1"/>
-      <c r="D288" s="1"/>
-      <c r="E288" s="1"/>
-    </row>
-    <row r="289" spans="1:5">
+    </row>
+    <row r="289" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A289" s="1"/>
       <c r="C289" s="1"/>
-      <c r="D289" s="1"/>
-      <c r="E289" s="1"/>
-    </row>
-    <row r="290" spans="1:5">
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A290" s="1"/>
       <c r="C290" s="1"/>
-      <c r="D290" s="1"/>
-      <c r="E290" s="1"/>
-    </row>
-    <row r="291" spans="1:5">
+    </row>
+    <row r="291" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A291" s="1"/>
       <c r="C291" s="1"/>
     </row>
-    <row r="292" spans="1:5">
+    <row r="292" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A292" s="1"/>
       <c r="C292" s="1"/>
     </row>
-    <row r="293" spans="1:5">
+    <row r="293" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A293" s="1"/>
       <c r="C293" s="1"/>
     </row>
-    <row r="294" spans="1:5">
+    <row r="294" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A294" s="1"/>
       <c r="C294" s="1"/>
     </row>
-    <row r="295" spans="1:5">
+    <row r="295" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A295" s="1"/>
       <c r="C295" s="1"/>
     </row>
-    <row r="296" spans="1:5">
+    <row r="296" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A296" s="1"/>
       <c r="C296" s="1"/>
     </row>
-    <row r="297" spans="1:5">
+    <row r="297" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A297" s="1"/>
       <c r="C297" s="1"/>
     </row>
-    <row r="298" spans="1:5">
+    <row r="298" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A298" s="1"/>
       <c r="C298" s="1"/>
     </row>
-    <row r="299" spans="1:5">
+    <row r="299" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A299" s="1"/>
       <c r="C299" s="1"/>
     </row>
-    <row r="300" spans="1:5">
+    <row r="300" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A300" s="1"/>
       <c r="C300" s="1"/>
     </row>
-    <row r="301" spans="1:5">
+    <row r="301" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A301" s="1"/>
       <c r="C301" s="1"/>
     </row>
-    <row r="302" spans="1:5">
+    <row r="302" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A302" s="1"/>
       <c r="C302" s="1"/>
     </row>
-    <row r="303" spans="1:5">
+    <row r="303" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A303" s="1"/>
       <c r="C303" s="1"/>
     </row>
-    <row r="304" spans="1:5">
+    <row r="304" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A304" s="1"/>
       <c r="C304" s="1"/>
     </row>
-    <row r="305" spans="1:3">
+    <row r="305" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A305" s="1"/>
       <c r="C305" s="1"/>
     </row>
-    <row r="306" spans="1:3">
+    <row r="306" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A306" s="1"/>
       <c r="C306" s="1"/>
     </row>
-    <row r="307" spans="1:3">
+    <row r="307" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A307" s="1"/>
       <c r="C307" s="1"/>
     </row>
-    <row r="308" spans="1:3">
+    <row r="308" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A308" s="1"/>
       <c r="C308" s="1"/>
     </row>
-    <row r="309" spans="1:3">
+    <row r="309" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A309" s="1"/>
       <c r="C309" s="1"/>
     </row>
-    <row r="310" spans="1:3">
+    <row r="310" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A310" s="1"/>
       <c r="C310" s="1"/>
     </row>
-    <row r="311" spans="1:3">
+    <row r="311" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A311" s="1"/>
       <c r="C311" s="1"/>
     </row>
-    <row r="312" spans="1:3">
+    <row r="312" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A312" s="1"/>
       <c r="C312" s="1"/>
     </row>
-    <row r="313" spans="1:3">
+    <row r="313" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A313" s="1"/>
       <c r="C313" s="1"/>
     </row>
-    <row r="314" spans="1:3">
+    <row r="314" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A314" s="1"/>
       <c r="C314" s="1"/>
     </row>
-    <row r="315" spans="1:3">
+    <row r="315" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A315" s="1"/>
       <c r="C315" s="1"/>
     </row>
-    <row r="316" spans="1:3">
+    <row r="316" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A316" s="1"/>
       <c r="C316" s="1"/>
     </row>
-    <row r="317" spans="1:3">
+    <row r="317" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A317" s="1"/>
       <c r="C317" s="1"/>
     </row>
-    <row r="318" spans="1:3">
+    <row r="318" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A318" s="1"/>
       <c r="C318" s="1"/>
     </row>
-    <row r="319" spans="1:3">
+    <row r="319" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A319" s="1"/>
       <c r="C319" s="1"/>
     </row>
-    <row r="320" spans="1:3">
+    <row r="320" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A320" s="1"/>
       <c r="C320" s="1"/>
     </row>
-    <row r="321" spans="1:3">
+    <row r="321" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A321" s="1"/>
       <c r="C321" s="1"/>
     </row>
-    <row r="322" spans="1:3">
+    <row r="322" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A322" s="1"/>
       <c r="C322" s="1"/>
     </row>
-    <row r="323" spans="1:3">
+    <row r="323" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A323" s="1"/>
       <c r="C323" s="1"/>
     </row>
-    <row r="324" spans="1:3">
+    <row r="324" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A324" s="1"/>
       <c r="C324" s="1"/>
     </row>
-    <row r="325" spans="1:3">
+    <row r="325" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A325" s="1"/>
       <c r="C325" s="1"/>
     </row>
-    <row r="326" spans="1:3">
+    <row r="326" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A326" s="1"/>
       <c r="C326" s="1"/>
     </row>
-    <row r="327" spans="1:3">
+    <row r="327" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A327" s="1"/>
       <c r="C327" s="1"/>
     </row>
-    <row r="328" spans="1:3">
+    <row r="328" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A328" s="1"/>
       <c r="C328" s="1"/>
     </row>
-    <row r="329" spans="1:3">
+    <row r="329" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A329" s="1"/>
       <c r="C329" s="1"/>
     </row>
-    <row r="330" spans="1:3">
+    <row r="330" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A330" s="1"/>
       <c r="C330" s="1"/>
     </row>
-    <row r="331" spans="1:3">
+    <row r="331" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A331" s="1"/>
       <c r="C331" s="1"/>
     </row>
-    <row r="332" spans="1:3">
+    <row r="332" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A332" s="1"/>
       <c r="C332" s="1"/>
     </row>
-    <row r="333" spans="1:3">
+    <row r="333" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A333" s="1"/>
       <c r="C333" s="1"/>
     </row>
-    <row r="334" spans="1:3">
+    <row r="334" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A334" s="1"/>
       <c r="C334" s="1"/>
     </row>
-    <row r="335" spans="1:3">
+    <row r="335" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A335" s="1"/>
       <c r="C335" s="1"/>
     </row>
-    <row r="336" spans="1:3">
+    <row r="336" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A336" s="1"/>
       <c r="C336" s="1"/>
     </row>
-    <row r="337" spans="1:3">
+    <row r="337" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A337" s="1"/>
       <c r="C337" s="1"/>
     </row>
-    <row r="338" spans="1:3">
+    <row r="338" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A338" s="1"/>
       <c r="C338" s="1"/>
     </row>
-    <row r="339" spans="1:3">
+    <row r="339" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A339" s="1"/>
       <c r="C339" s="1"/>
     </row>
-    <row r="340" spans="1:3">
+    <row r="340" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A340" s="1"/>
       <c r="C340" s="1"/>
     </row>
-    <row r="341" spans="1:3">
+    <row r="341" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A341" s="1"/>
       <c r="C341" s="1"/>
     </row>
-    <row r="342" spans="1:3">
+    <row r="342" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A342" s="1"/>
       <c r="C342" s="1"/>
     </row>
-    <row r="343" spans="1:3">
+    <row r="343" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A343" s="1"/>
       <c r="C343" s="1"/>
     </row>
-    <row r="344" spans="1:3">
+    <row r="344" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A344" s="1"/>
       <c r="C344" s="1"/>
     </row>
-    <row r="345" spans="1:3">
+    <row r="345" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A345" s="1"/>
       <c r="C345" s="1"/>
     </row>
-    <row r="346" spans="1:3">
+    <row r="346" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A346" s="1"/>
       <c r="C346" s="1"/>
     </row>
-    <row r="347" spans="1:3">
+    <row r="347" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A347" s="1"/>
       <c r="C347" s="1"/>
     </row>
-    <row r="348" spans="1:3">
+    <row r="348" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A348" s="1"/>
       <c r="C348" s="1"/>
     </row>
-    <row r="349" spans="1:3">
+    <row r="349" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A349" s="1"/>
       <c r="C349" s="1"/>
     </row>
-    <row r="350" spans="1:3">
+    <row r="350" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A350" s="1"/>
       <c r="C350" s="1"/>
     </row>
-    <row r="351" spans="1:3">
+    <row r="351" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A351" s="1"/>
       <c r="C351" s="1"/>
     </row>
-    <row r="352" spans="1:3">
+    <row r="352" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A352" s="1"/>
       <c r="C352" s="1"/>
     </row>
-    <row r="353" spans="1:3">
+    <row r="353" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A353" s="1"/>
       <c r="C353" s="1"/>
     </row>
-    <row r="354" spans="1:3">
+    <row r="354" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A354" s="1"/>
       <c r="C354" s="1"/>
     </row>
-    <row r="355" spans="1:3">
+    <row r="355" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A355" s="1"/>
       <c r="C355" s="1"/>
     </row>
-    <row r="356" spans="1:3">
+    <row r="356" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A356" s="1"/>
       <c r="C356" s="1"/>
     </row>
-    <row r="357" spans="1:3">
+    <row r="357" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A357" s="1"/>
       <c r="C357" s="1"/>
     </row>
-    <row r="358" spans="1:3">
+    <row r="358" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A358" s="1"/>
       <c r="C358" s="1"/>
     </row>
-    <row r="359" spans="1:3">
+    <row r="359" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A359" s="1"/>
       <c r="C359" s="1"/>
     </row>
-    <row r="360" spans="1:3">
+    <row r="360" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A360" s="1"/>
       <c r="C360" s="1"/>
     </row>
-    <row r="361" spans="1:3">
+    <row r="361" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A361" s="1"/>
       <c r="C361" s="1"/>
     </row>
-    <row r="362" spans="1:3">
+    <row r="362" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A362" s="1"/>
       <c r="C362" s="1"/>
     </row>
-    <row r="363" spans="1:3">
+    <row r="363" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A363" s="1"/>
       <c r="C363" s="1"/>
     </row>
-    <row r="364" spans="1:3">
+    <row r="364" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A364" s="1"/>
       <c r="C364" s="1"/>
     </row>
-    <row r="365" spans="1:3">
+    <row r="365" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A365" s="1"/>
       <c r="C365" s="1"/>
     </row>
-    <row r="366" spans="1:3">
+    <row r="366" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A366" s="1"/>
       <c r="C366" s="1"/>
     </row>
-    <row r="367" spans="1:3">
+    <row r="367" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A367" s="1"/>
       <c r="C367" s="1"/>
     </row>
-    <row r="368" spans="1:3">
+    <row r="368" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A368" s="1"/>
       <c r="C368" s="1"/>
     </row>
-    <row r="369" spans="1:3">
+    <row r="369" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A369" s="1"/>
       <c r="C369" s="1"/>
     </row>
-    <row r="370" spans="1:3">
+    <row r="370" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A370" s="1"/>
       <c r="C370" s="1"/>
     </row>
-    <row r="371" spans="1:3">
+    <row r="371" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A371" s="1"/>
       <c r="C371" s="1"/>
     </row>
-    <row r="372" spans="1:3">
+    <row r="372" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A372" s="1"/>
       <c r="C372" s="1"/>
     </row>
-    <row r="373" spans="1:3">
+    <row r="373" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A373" s="1"/>
       <c r="C373" s="1"/>
     </row>
-    <row r="374" spans="1:3">
+    <row r="374" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A374" s="1"/>
       <c r="C374" s="1"/>
     </row>
-    <row r="375" spans="1:3">
+    <row r="375" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A375" s="1"/>
       <c r="C375" s="1"/>
     </row>
-    <row r="376" spans="1:3">
+    <row r="376" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A376" s="1"/>
       <c r="C376" s="1"/>
     </row>
-    <row r="377" spans="1:3">
+    <row r="377" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A377" s="1"/>
       <c r="C377" s="1"/>
     </row>
-    <row r="378" spans="1:3">
+    <row r="378" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A378" s="1"/>
       <c r="C378" s="1"/>
     </row>
-    <row r="379" spans="1:3">
+    <row r="379" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A379" s="1"/>
       <c r="C379" s="1"/>
     </row>
-    <row r="380" spans="1:3">
+    <row r="380" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A380" s="1"/>
       <c r="C380" s="1"/>
     </row>
-    <row r="381" spans="1:3">
+    <row r="381" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A381" s="1"/>
       <c r="C381" s="1"/>
     </row>
-    <row r="382" spans="1:3">
+    <row r="382" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A382" s="1"/>
       <c r="C382" s="1"/>
     </row>
-    <row r="383" spans="1:3">
+    <row r="383" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A383" s="1"/>
       <c r="C383" s="1"/>
     </row>
-    <row r="384" spans="1:3">
+    <row r="384" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A384" s="1"/>
       <c r="C384" s="1"/>
     </row>
-    <row r="385" spans="1:3">
+    <row r="385" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A385" s="1"/>
       <c r="C385" s="1"/>
     </row>
-    <row r="386" spans="1:3">
+    <row r="386" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A386" s="1"/>
       <c r="C386" s="1"/>
     </row>
-    <row r="387" spans="1:3">
+    <row r="387" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A387" s="1"/>
       <c r="C387" s="1"/>
     </row>
-    <row r="388" spans="1:3">
+    <row r="388" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A388" s="1"/>
       <c r="C388" s="1"/>
     </row>
-    <row r="389" spans="1:3">
+    <row r="389" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A389" s="1"/>
       <c r="C389" s="1"/>
     </row>
-    <row r="390" spans="1:3">
+    <row r="390" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A390" s="1"/>
       <c r="C390" s="1"/>
     </row>
-    <row r="391" spans="1:3">
+    <row r="391" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A391" s="1"/>
       <c r="C391" s="1"/>
     </row>
-    <row r="392" spans="1:3">
+    <row r="392" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A392" s="1"/>
       <c r="C392" s="1"/>
     </row>
-    <row r="393" spans="1:3">
+    <row r="393" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A393" s="1"/>
       <c r="C393" s="1"/>
     </row>
-    <row r="394" spans="1:3">
+    <row r="394" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A394" s="1"/>
       <c r="C394" s="1"/>
     </row>
-    <row r="395" spans="1:3">
+    <row r="395" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A395" s="1"/>
       <c r="C395" s="1"/>
     </row>
-    <row r="396" spans="1:3">
+    <row r="396" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A396" s="1"/>
       <c r="C396" s="1"/>
     </row>
-    <row r="397" spans="1:3">
+    <row r="397" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A397" s="1"/>
       <c r="C397" s="1"/>
     </row>
-    <row r="398" spans="1:3">
+    <row r="398" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A398" s="1"/>
       <c r="C398" s="1"/>
     </row>
-    <row r="399" spans="1:3">
+    <row r="399" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A399" s="1"/>
       <c r="C399" s="1"/>
     </row>
-    <row r="400" spans="1:3">
+    <row r="400" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A400" s="1"/>
       <c r="C400" s="1"/>
     </row>
-    <row r="401" spans="1:3">
+    <row r="401" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A401" s="1"/>
       <c r="C401" s="1"/>
     </row>
-    <row r="402" spans="1:3">
+    <row r="402" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A402" s="1"/>
       <c r="C402" s="1"/>
     </row>
-    <row r="403" spans="1:3">
+    <row r="403" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A403" s="1"/>
       <c r="C403" s="1"/>
     </row>
-    <row r="404" spans="1:3">
+    <row r="404" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A404" s="1"/>
       <c r="C404" s="1"/>
     </row>
-    <row r="405" spans="1:3">
+    <row r="405" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A405" s="1"/>
       <c r="C405" s="1"/>
     </row>
-    <row r="406" spans="1:3">
+    <row r="406" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A406" s="1"/>
       <c r="C406" s="1"/>
     </row>
-    <row r="407" spans="1:3">
+    <row r="407" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A407" s="1"/>
       <c r="C407" s="1"/>
-    </row>
-    <row r="408" spans="1:3">
-      <c r="A408" s="1"/>
-      <c r="C408" s="1"/>
-    </row>
-    <row r="409" spans="1:3">
-      <c r="A409" s="1"/>
-      <c r="C409" s="1"/>
-    </row>
-    <row r="410" spans="1:3">
-      <c r="A410" s="1"/>
-      <c r="C410" s="1"/>
-    </row>
-    <row r="411" spans="1:3">
-      <c r="A411" s="1"/>
-      <c r="C411" s="1"/>
-    </row>
-    <row r="412" spans="1:3">
-      <c r="A412" s="1"/>
-      <c r="C412" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4876,7 +4765,203 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CC4A59B-2E01-A945-BEC9-26E74186C39C}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="160" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="1">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="224" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="1">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="272" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="1">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="380" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="1">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8781A4A4-58ED-1144-B4A4-C7E6398DC6EB}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="395" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="1">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="1">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="1">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="009352bb-e01b-434b-b557-66f85abfe1dc" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8632a450-842f-4271-a6e0-618a8be3193b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Asiakirja" ma:contentTypeID="0x01010085C762B25A797648B7B0C4F73DAF4C4E" ma:contentTypeVersion="12" ma:contentTypeDescription="Luo uusi asiakirja." ma:contentTypeScope="" ma:versionID="85fcd9168920706c1ab8cb9a512a824a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="8632a450-842f-4271-a6e0-618a8be3193b" xmlns:ns3="009352bb-e01b-434b-b557-66f85abfe1dc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="40dc8aa416c75f6f0d5c7355293e8cbe" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5082,19 +5167,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="009352bb-e01b-434b-b557-66f85abfe1dc" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8632a450-842f-4271-a6e0-618a8be3193b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -5105,15 +5177,43 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C2846B4-9390-4622-9FF7-6E5B130FE615}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D0897DE-87B6-4870-8A11-64380A3B85DD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="009352bb-e01b-434b-b557-66f85abfe1dc"/>
+    <ds:schemaRef ds:uri="8632a450-842f-4271-a6e0-618a8be3193b"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D0897DE-87B6-4870-8A11-64380A3B85DD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C2846B4-9390-4622-9FF7-6E5B130FE615}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="8632a450-842f-4271-a6e0-618a8be3193b"/>
+    <ds:schemaRef ds:uri="009352bb-e01b-434b-b557-66f85abfe1dc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE7BE5DD-B990-4EA4-A131-1D341433C869}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE7BE5DD-B990-4EA4-A131-1D341433C869}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>